<commit_message>
Marginal VAR addition and updates
Added the marginal var function and updated tests and other functionality
</commit_message>
<xml_diff>
--- a/docs/Portfolio_VAR.xlsx
+++ b/docs/Portfolio_VAR.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\python_packages\pyFinRisk\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DCF0693-4C4F-445F-9F23-EC2D036C14BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D30E1AA-C0EF-46D1-A265-00B074B0AD1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="2310" windowWidth="29040" windowHeight="16440" xr2:uid="{4B25372F-870B-4A45-8A4D-D63FBB30CA3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Portfolio VAR" sheetId="1" r:id="rId1"/>
-    <sheet name="JPM Data" sheetId="2" r:id="rId2"/>
-    <sheet name="NVDA Data" sheetId="3" r:id="rId3"/>
-    <sheet name="LLY Data" sheetId="4" r:id="rId4"/>
+    <sheet name="SPY Data" sheetId="5" r:id="rId2"/>
+    <sheet name="JPM Data" sheetId="2" r:id="rId3"/>
+    <sheet name="NVDA Data" sheetId="3" r:id="rId4"/>
+    <sheet name="LLY Data" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="26">
   <si>
     <t>Holdings</t>
   </si>
@@ -133,6 +134,12 @@
   </si>
   <si>
     <t>Individual VAR ($)</t>
+  </si>
+  <si>
+    <t>Beta</t>
+  </si>
+  <si>
+    <t>SPY</t>
   </si>
 </sst>
 </file>
@@ -258,7 +265,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -273,16 +280,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -630,7 +631,7 @@
   <dimension ref="A1:N269"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,7 +664,7 @@
       <c r="C2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -806,42 +807,42 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="18">
+      <c r="B6" s="12">
         <f>SUM(B3:B5)</f>
         <v>1</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="12">
         <v>6000</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="17">
         <f>SUM(D3:D5)</f>
         <v>2752430.0537109366</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6">
         <v>7.4974003262044485E-6</v>
       </c>
-      <c r="G6" s="17">
+      <c r="G6">
         <v>1.302962560624621E-4</v>
       </c>
-      <c r="H6" s="17">
+      <c r="H6">
         <f>VARP('Portfolio VAR'!$D$18:$D$269)</f>
         <v>3.5365141235931972E-4</v>
       </c>
-      <c r="J6" s="21" t="s">
+      <c r="J6" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="K6" s="22">
+      <c r="K6" s="16">
         <f>K3*K5</f>
         <v>3.6805275587015122E-2</v>
       </c>
-      <c r="L6" s="22">
+      <c r="L6" s="16">
         <f t="shared" ref="L6:M6" si="0">L3*L5</f>
         <v>2.6063821767628736E-2</v>
       </c>
-      <c r="M6" s="22">
+      <c r="M6" s="16">
         <f t="shared" si="0"/>
         <v>2.0219207189433201E-2</v>
       </c>
@@ -850,18 +851,18 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
     </row>
     <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="6" t="s">
         <v>15</v>
       </c>
       <c r="J8" t="s">
@@ -885,7 +886,7 @@
       <c r="G9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="H9" s="11" t="s">
         <v>4</v>
       </c>
       <c r="J9" s="9" t="s">
@@ -905,14 +906,14 @@
       <c r="E10" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10">
         <f>VARP('Portfolio VAR'!$F$18:$F$269)</f>
         <v>2.0491418582103136E-5</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10">
         <v>9.883259668719173E-6</v>
       </c>
-      <c r="H10" s="15">
+      <c r="H10" s="12">
         <v>1.4815129873943736E-6</v>
       </c>
       <c r="J10" t="s">
@@ -935,14 +936,14 @@
       <c r="E11" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11">
         <v>9.883259668719173E-6</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11">
         <f>VARP('Portfolio VAR'!$G$18:$G$269)</f>
         <v>1.7130394784964511E-4</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11">
         <v>2.4400340678834549E-5</v>
       </c>
       <c r="I11" s="8"/>
@@ -966,28 +967,28 @@
       <c r="E12" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F12" s="13">
+      <c r="F12" s="10">
         <v>1.4815129873943736E-6</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G12" s="10">
         <v>2.4400340678834549E-5</v>
       </c>
-      <c r="H12" s="13">
+      <c r="H12" s="10">
         <f>VARP('Portfolio VAR'!$H$18:$H$269)</f>
         <v>6.4167171185979682E-5</v>
       </c>
-      <c r="J12" s="19" t="s">
+      <c r="J12" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="K12" s="20">
+      <c r="K12" s="14">
         <f>K9*K11</f>
         <v>1.5644169602477314E-2</v>
       </c>
-      <c r="L12" s="20">
-        <f t="shared" ref="L12:M12" si="2">L9*L11</f>
+      <c r="L12" s="14">
+        <f t="shared" ref="L12" si="2">L9*L11</f>
         <v>1.107848920347106E-2</v>
       </c>
-      <c r="M12" s="20">
+      <c r="M12" s="14">
         <f>M9*M11</f>
         <v>8.5942219275411853E-3</v>
       </c>
@@ -996,6 +997,21 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14">
+        <f>SLOPE(_xlfn.ANCHORARRAY(B18),'SPY Data'!$C$3:$C$254)</f>
+        <v>0.71734466408875841</v>
+      </c>
+      <c r="C14">
+        <f>SLOPE(_xlfn.ANCHORARRAY(C18),'SPY Data'!$C$3:$C$254)</f>
+        <v>2.3843784827265293</v>
+      </c>
+      <c r="D14">
+        <f>SLOPE(_xlfn.ANCHORARRAY(D18),'SPY Data'!$C$3:$C$254)</f>
+        <v>0.59978867061257335</v>
+      </c>
       <c r="J14" s="1" t="s">
         <v>21</v>
       </c>
@@ -1018,7 +1034,7 @@
         <v>1.0404111650873007E-2</v>
       </c>
       <c r="C15">
-        <f t="shared" ref="C15:H15" si="3">_xlfn.STDEV.S(_xlfn.ANCHORARRAY(C18))</f>
+        <f t="shared" ref="C15" si="3">_xlfn.STDEV.S(_xlfn.ANCHORARRAY(C18))</f>
         <v>3.1207322587394754E-2</v>
       </c>
       <c r="D15">
@@ -1040,7 +1056,7 @@
       <c r="J15" t="s">
         <v>16</v>
       </c>
-      <c r="K15" s="24">
+      <c r="K15" s="18">
         <f>$D$6*K6</f>
         <v>101303.94666081386</v>
       </c>
@@ -1063,15 +1079,15 @@
       <c r="J16" t="s">
         <v>17</v>
       </c>
-      <c r="K16" s="24">
+      <c r="K16" s="18">
         <f>$D$6*K12</f>
         <v>43059.482579209638</v>
       </c>
-      <c r="L16" s="24">
+      <c r="L16" s="18">
         <f t="shared" ref="L16:M16" si="6">$D$6*L12</f>
         <v>30492.76663334588</v>
       </c>
-      <c r="M16" s="24">
+      <c r="M16" s="18">
         <f t="shared" si="6"/>
         <v>23654.994721625895</v>
       </c>
@@ -1086,16 +1102,16 @@
       <c r="D17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="H17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K17" s="10"/>
+      <c r="K17" s="6"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="4" cm="1">
@@ -1160,15 +1176,15 @@
       <c r="J19" t="s">
         <v>2</v>
       </c>
-      <c r="K19" s="25">
+      <c r="K19" s="19">
         <f>$B$15*K18*$B$3</f>
         <v>4.0483438844711962E-3</v>
       </c>
-      <c r="L19" s="25">
+      <c r="L19" s="19">
         <f t="shared" ref="L19:M19" si="7">$B$15*L18*$B$3</f>
         <v>2.8668529653980571E-3</v>
       </c>
-      <c r="M19" s="25">
+      <c r="M19" s="19">
         <f t="shared" si="7"/>
         <v>2.2239829064906141E-3</v>
       </c>
@@ -1198,15 +1214,15 @@
       <c r="J20" t="s">
         <v>3</v>
       </c>
-      <c r="K20" s="25">
+      <c r="K20" s="19">
         <f>$C$15*$B$4*K18</f>
         <v>2.4213449522333716E-2</v>
       </c>
-      <c r="L20" s="25">
+      <c r="L20" s="19">
         <f t="shared" ref="L20:M20" si="8">$C$15*$B$4*L18</f>
         <v>1.7146863395644047E-2</v>
       </c>
-      <c r="M20" s="25">
+      <c r="M20" s="19">
         <f t="shared" si="8"/>
         <v>1.3301809179651141E-2</v>
       </c>
@@ -1236,15 +1252,15 @@
       <c r="J21" t="s">
         <v>4</v>
       </c>
-      <c r="K21" s="25">
+      <c r="K21" s="19">
         <f>$D$15*$B$5*K18</f>
         <v>2.1952148576755513E-2</v>
       </c>
-      <c r="L21" s="25">
+      <c r="L21" s="19">
         <f t="shared" ref="L21:M21" si="9">$D$15*$B$5*L18</f>
         <v>1.5545512940620855E-2</v>
       </c>
-      <c r="M21" s="25">
+      <c r="M21" s="19">
         <f t="shared" si="9"/>
         <v>1.2059549432724057E-2</v>
       </c>
@@ -1332,15 +1348,15 @@
       <c r="J24" t="s">
         <v>2</v>
       </c>
-      <c r="K24" s="24">
+      <c r="K24" s="18">
         <f>$B$15*K23*$C$3*'JPM Data'!$B$254</f>
         <v>4899.4657782118802</v>
       </c>
-      <c r="L24" s="24">
+      <c r="L24" s="18">
         <f>$B$15*L23*$C$3*'JPM Data'!$B$254</f>
         <v>3469.5787699783705</v>
       </c>
-      <c r="M24" s="24">
+      <c r="M24" s="18">
         <f>$B$15*M23*$C$3*'JPM Data'!$B$254</f>
         <v>2691.5520154983724</v>
       </c>
@@ -1370,15 +1386,15 @@
       <c r="J25" t="s">
         <v>3</v>
       </c>
-      <c r="K25" s="24">
+      <c r="K25" s="18">
         <f>$C$15*K23*$C$4*'NVDA Data'!$B$254</f>
         <v>13761.673644409686</v>
       </c>
-      <c r="L25" s="24">
+      <c r="L25" s="18">
         <f>$C$15*L23*$C$4*'NVDA Data'!$B$254</f>
         <v>9745.3912074145828</v>
       </c>
-      <c r="M25" s="24">
+      <c r="M25" s="18">
         <f>$C$15*M23*$C$4*'NVDA Data'!$B$254</f>
         <v>7560.0610578731312</v>
       </c>
@@ -1408,15 +1424,15 @@
       <c r="J26" t="s">
         <v>4</v>
       </c>
-      <c r="K26" s="24">
+      <c r="K26" s="18">
         <f>$D$15*K23*$C$5*'LLY Data'!$B$254</f>
         <v>103660.68240978617</v>
       </c>
-      <c r="L26" s="24">
+      <c r="L26" s="18">
         <f>$D$15*L23*$C$5*'LLY Data'!$B$254</f>
         <v>73407.779388904353</v>
       </c>
-      <c r="M26" s="24">
+      <c r="M26" s="18">
         <f>$D$15*M23*$C$5*'LLY Data'!$B$254</f>
         <v>56946.640980483375</v>
       </c>
@@ -7017,11 +7033,3072 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A10429B7-D921-4878-B446-8F94187785FF}">
+  <dimension ref="A1:C254"/>
+  <sheetViews>
+    <sheetView topLeftCell="A217" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C254"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>45061</v>
+      </c>
+      <c r="B2">
+        <v>413.01001000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>45062</v>
+      </c>
+      <c r="B3">
+        <v>410.25</v>
+      </c>
+      <c r="C3">
+        <f>B3/B2-1</f>
+        <v>-6.6826709599605572E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>45063</v>
+      </c>
+      <c r="B4">
+        <v>415.23001099999999</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C67" si="0">B4/B3-1</f>
+        <v>1.2138966483851377E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>45064</v>
+      </c>
+      <c r="B5">
+        <v>419.23001099999999</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>9.6332150712488129E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>45065</v>
+      </c>
+      <c r="B6">
+        <v>418.61999500000002</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>-1.4550866684016617E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>45068</v>
+      </c>
+      <c r="B7">
+        <v>418.790009</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>4.0612966898523339E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>45069</v>
+      </c>
+      <c r="B8">
+        <v>414.08999599999999</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>-1.1222839368166482E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>45070</v>
+      </c>
+      <c r="B9">
+        <v>411.08999599999999</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>-7.2448019246521556E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>45071</v>
+      </c>
+      <c r="B10">
+        <v>414.64999399999999</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>8.6598993763886689E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>45072</v>
+      </c>
+      <c r="B11">
+        <v>420.01998900000001</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>1.2950669426514017E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>45076</v>
+      </c>
+      <c r="B12">
+        <v>420.17999300000002</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>3.8094377455921702E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>45077</v>
+      </c>
+      <c r="B13">
+        <v>417.85000600000001</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>-5.5452116683718522E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>45078</v>
+      </c>
+      <c r="B14">
+        <v>421.82000699999998</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>9.5010193681797084E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>45079</v>
+      </c>
+      <c r="B15">
+        <v>427.92001299999998</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>1.4461158548129349E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>45082</v>
+      </c>
+      <c r="B16">
+        <v>427.10000600000001</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>-1.9162623272774848E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>45083</v>
+      </c>
+      <c r="B17">
+        <v>428.02999899999998</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>2.1774595807426689E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>45084</v>
+      </c>
+      <c r="B18">
+        <v>426.54998799999998</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>-3.4577272701860062E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>45085</v>
+      </c>
+      <c r="B19">
+        <v>429.13000499999998</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>6.048568919429842E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>45086</v>
+      </c>
+      <c r="B20">
+        <v>429.89999399999999</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>1.7943024049320577E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>45089</v>
+      </c>
+      <c r="B21">
+        <v>433.79998799999998</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>9.0718633506190471E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>45090</v>
+      </c>
+      <c r="B22">
+        <v>436.66000400000001</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>6.5929370196295967E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>45091</v>
+      </c>
+      <c r="B23">
+        <v>437.17999300000002</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>1.1908326735599051E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>45092</v>
+      </c>
+      <c r="B24">
+        <v>442.60000600000001</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>1.239766935080211E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>45093</v>
+      </c>
+      <c r="B25">
+        <v>439.459991</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>-7.0944757284978621E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>45097</v>
+      </c>
+      <c r="B26">
+        <v>437.17999300000002</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>-5.1881810555991503E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>45098</v>
+      </c>
+      <c r="B27">
+        <v>434.94000199999999</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>-5.1237271509815274E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>45099</v>
+      </c>
+      <c r="B28">
+        <v>436.51001000000002</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>3.6097116677715757E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>45100</v>
+      </c>
+      <c r="B29">
+        <v>433.209991</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>-7.5600076158620633E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>45103</v>
+      </c>
+      <c r="B30">
+        <v>431.44000199999999</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>-4.085752953006172E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>45104</v>
+      </c>
+      <c r="B31">
+        <v>436.17001299999998</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>1.0963311185966385E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>45105</v>
+      </c>
+      <c r="B32">
+        <v>436.39001500000001</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>5.0439506028121528E-4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>45106</v>
+      </c>
+      <c r="B33">
+        <v>438.10998499999999</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>3.9413596573698584E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>45107</v>
+      </c>
+      <c r="B34">
+        <v>443.27999899999998</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>1.1800721684076532E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>45110</v>
+      </c>
+      <c r="B35">
+        <v>443.790009</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>1.1505369092910112E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>45112</v>
+      </c>
+      <c r="B36">
+        <v>443.13000499999998</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>-1.4871988702206407E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>45113</v>
+      </c>
+      <c r="B37">
+        <v>439.66000400000001</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>-7.8306613428263949E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>45114</v>
+      </c>
+      <c r="B38">
+        <v>438.54998799999998</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>-2.5247145291843465E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>45117</v>
+      </c>
+      <c r="B39">
+        <v>439.66000400000001</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>2.5311048463647623E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>45118</v>
+      </c>
+      <c r="B40">
+        <v>442.459991</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>6.3685278954781488E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>45119</v>
+      </c>
+      <c r="B41">
+        <v>446.01998900000001</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>8.0459206988503507E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>45120</v>
+      </c>
+      <c r="B42">
+        <v>449.55999800000001</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>7.9368841919773558E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>45121</v>
+      </c>
+      <c r="B43">
+        <v>449.27999899999998</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>-6.228289911150986E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>45124</v>
+      </c>
+      <c r="B44">
+        <v>450.83999599999999</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>3.472215552600133E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>45125</v>
+      </c>
+      <c r="B45">
+        <v>454.19000199999999</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>7.4305874139879435E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>45126</v>
+      </c>
+      <c r="B46">
+        <v>455.20001200000002</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>2.2237609712949524E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>45127</v>
+      </c>
+      <c r="B47">
+        <v>452.17999300000002</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>-6.6344879621839103E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>45128</v>
+      </c>
+      <c r="B48">
+        <v>452.17999300000002</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>45131</v>
+      </c>
+      <c r="B49">
+        <v>454.20001200000002</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="0"/>
+        <v>4.4672896441042553E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>45132</v>
+      </c>
+      <c r="B50">
+        <v>455.44000199999999</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="0"/>
+        <v>2.7300527680302888E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>45133</v>
+      </c>
+      <c r="B51">
+        <v>455.51001000000002</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="0"/>
+        <v>1.53715088030415E-4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <v>45134</v>
+      </c>
+      <c r="B52">
+        <v>452.48998999999998</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="0"/>
+        <v>-6.6299750470907304E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
+        <v>45135</v>
+      </c>
+      <c r="B53">
+        <v>456.92001299999998</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="0"/>
+        <v>9.7903226544304722E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
+        <v>45138</v>
+      </c>
+      <c r="B54">
+        <v>457.790009</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="0"/>
+        <v>1.9040444175073556E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
+        <v>45139</v>
+      </c>
+      <c r="B55">
+        <v>456.48001099999999</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="0"/>
+        <v>-2.8615696591142159E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
+        <v>45140</v>
+      </c>
+      <c r="B56">
+        <v>450.13000499999998</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="0"/>
+        <v>-1.391080846254189E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
+        <v>45141</v>
+      </c>
+      <c r="B57">
+        <v>448.83999599999999</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="0"/>
+        <v>-2.8658587200823815E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
+        <v>45142</v>
+      </c>
+      <c r="B58">
+        <v>446.80999800000001</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="0"/>
+        <v>-4.5227653909879484E-3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
+        <v>45145</v>
+      </c>
+      <c r="B59">
+        <v>450.709991</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="0"/>
+        <v>8.7285267058863081E-3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
+        <v>45146</v>
+      </c>
+      <c r="B60">
+        <v>448.75</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="0"/>
+        <v>-4.3486744006968614E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
+        <v>45147</v>
+      </c>
+      <c r="B61">
+        <v>445.75</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="0"/>
+        <v>-6.6852367688022829E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
+        <v>45148</v>
+      </c>
+      <c r="B62">
+        <v>445.91000400000001</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="0"/>
+        <v>3.5895457094792249E-4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
+        <v>45149</v>
+      </c>
+      <c r="B63">
+        <v>445.64999399999999</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="0"/>
+        <v>-5.8309972341419325E-4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
+        <v>45152</v>
+      </c>
+      <c r="B64">
+        <v>448.10998499999999</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="0"/>
+        <v>5.520006806058575E-3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
+        <v>45153</v>
+      </c>
+      <c r="B65">
+        <v>442.89001500000001</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="0"/>
+        <v>-1.1648858929130923E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
+        <v>45154</v>
+      </c>
+      <c r="B66">
+        <v>439.64001500000001</v>
+      </c>
+      <c r="C66">
+        <f t="shared" si="0"/>
+        <v>-7.3381649843697883E-3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
+        <v>45155</v>
+      </c>
+      <c r="B67">
+        <v>436.290009</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="0"/>
+        <v>-7.6198841909329573E-3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
+        <v>45156</v>
+      </c>
+      <c r="B68">
+        <v>436.5</v>
+      </c>
+      <c r="C68">
+        <f t="shared" ref="C68:C131" si="1">B68/B67-1</f>
+        <v>4.8131058623446243E-4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="2">
+        <v>45159</v>
+      </c>
+      <c r="B69">
+        <v>439.33999599999999</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="1"/>
+        <v>6.5062909507445088E-3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="2">
+        <v>45160</v>
+      </c>
+      <c r="B70">
+        <v>438.14999399999999</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="1"/>
+        <v>-2.7086129440397899E-3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="2">
+        <v>45161</v>
+      </c>
+      <c r="B71">
+        <v>443.02999899999998</v>
+      </c>
+      <c r="C71">
+        <f t="shared" si="1"/>
+        <v>1.1137749781642059E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
+        <v>45162</v>
+      </c>
+      <c r="B72">
+        <v>436.89001500000001</v>
+      </c>
+      <c r="C72">
+        <f t="shared" si="1"/>
+        <v>-1.385907052312263E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
+        <v>45163</v>
+      </c>
+      <c r="B73">
+        <v>439.97000100000002</v>
+      </c>
+      <c r="C73">
+        <f t="shared" si="1"/>
+        <v>7.049797189803142E-3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="2">
+        <v>45166</v>
+      </c>
+      <c r="B74">
+        <v>442.76001000000002</v>
+      </c>
+      <c r="C74">
+        <f t="shared" si="1"/>
+        <v>6.341361896626152E-3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="2">
+        <v>45167</v>
+      </c>
+      <c r="B75">
+        <v>449.16000400000001</v>
+      </c>
+      <c r="C75">
+        <f t="shared" si="1"/>
+        <v>1.4454769752128227E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="2">
+        <v>45168</v>
+      </c>
+      <c r="B76">
+        <v>451.01001000000002</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="1"/>
+        <v>4.1188128585019079E-3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="2">
+        <v>45169</v>
+      </c>
+      <c r="B77">
+        <v>450.35000600000001</v>
+      </c>
+      <c r="C77">
+        <f t="shared" si="1"/>
+        <v>-1.4633910231837133E-3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="2">
+        <v>45170</v>
+      </c>
+      <c r="B78">
+        <v>451.19000199999999</v>
+      </c>
+      <c r="C78">
+        <f t="shared" si="1"/>
+        <v>1.8652070363245343E-3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="2">
+        <v>45174</v>
+      </c>
+      <c r="B79">
+        <v>449.23998999999998</v>
+      </c>
+      <c r="C79">
+        <f t="shared" si="1"/>
+        <v>-4.3219308747005636E-3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="2">
+        <v>45175</v>
+      </c>
+      <c r="B80">
+        <v>446.22000100000002</v>
+      </c>
+      <c r="C80">
+        <f t="shared" si="1"/>
+        <v>-6.7224402707335429E-3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="2">
+        <v>45176</v>
+      </c>
+      <c r="B81">
+        <v>444.85000600000001</v>
+      </c>
+      <c r="C81">
+        <f t="shared" si="1"/>
+        <v>-3.0702232014024888E-3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="2">
+        <v>45177</v>
+      </c>
+      <c r="B82">
+        <v>445.51998900000001</v>
+      </c>
+      <c r="C82">
+        <f t="shared" si="1"/>
+        <v>1.5060874248926659E-3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="2">
+        <v>45180</v>
+      </c>
+      <c r="B83">
+        <v>448.45001200000002</v>
+      </c>
+      <c r="C83">
+        <f t="shared" si="1"/>
+        <v>6.5766364525565724E-3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="2">
+        <v>45181</v>
+      </c>
+      <c r="B84">
+        <v>445.98998999999998</v>
+      </c>
+      <c r="C84">
+        <f t="shared" si="1"/>
+        <v>-5.4856102891576164E-3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="2">
+        <v>45182</v>
+      </c>
+      <c r="B85">
+        <v>446.51001000000002</v>
+      </c>
+      <c r="C85">
+        <f t="shared" si="1"/>
+        <v>1.1659902949840983E-3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="2">
+        <v>45183</v>
+      </c>
+      <c r="B86">
+        <v>450.35998499999999</v>
+      </c>
+      <c r="C86">
+        <f t="shared" si="1"/>
+        <v>8.6223710863726488E-3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="2">
+        <v>45184</v>
+      </c>
+      <c r="B87">
+        <v>443.36999500000002</v>
+      </c>
+      <c r="C87">
+        <f t="shared" si="1"/>
+        <v>-1.5520894912544159E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="2">
+        <v>45187</v>
+      </c>
+      <c r="B88">
+        <v>443.63000499999998</v>
+      </c>
+      <c r="C88">
+        <f t="shared" si="1"/>
+        <v>5.864402258433099E-4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="2">
+        <v>45188</v>
+      </c>
+      <c r="B89">
+        <v>442.709991</v>
+      </c>
+      <c r="C89">
+        <f t="shared" si="1"/>
+        <v>-2.0738317733940415E-3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="2">
+        <v>45189</v>
+      </c>
+      <c r="B90">
+        <v>438.64001500000001</v>
+      </c>
+      <c r="C90">
+        <f t="shared" si="1"/>
+        <v>-9.1933231296783546E-3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="2">
+        <v>45190</v>
+      </c>
+      <c r="B91">
+        <v>431.39001500000001</v>
+      </c>
+      <c r="C91">
+        <f t="shared" si="1"/>
+        <v>-1.6528359821435856E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="2">
+        <v>45191</v>
+      </c>
+      <c r="B92">
+        <v>430.42001299999998</v>
+      </c>
+      <c r="C92">
+        <f t="shared" si="1"/>
+        <v>-2.2485499577453716E-3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="2">
+        <v>45194</v>
+      </c>
+      <c r="B93">
+        <v>432.23001099999999</v>
+      </c>
+      <c r="C93">
+        <f t="shared" si="1"/>
+        <v>4.2051901522526247E-3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="2">
+        <v>45195</v>
+      </c>
+      <c r="B94">
+        <v>425.88000499999998</v>
+      </c>
+      <c r="C94">
+        <f t="shared" si="1"/>
+        <v>-1.4691265850117041E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="2">
+        <v>45196</v>
+      </c>
+      <c r="B95">
+        <v>426.04998799999998</v>
+      </c>
+      <c r="C95">
+        <f t="shared" si="1"/>
+        <v>3.9913355406295814E-4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="2">
+        <v>45197</v>
+      </c>
+      <c r="B96">
+        <v>428.51998900000001</v>
+      </c>
+      <c r="C96">
+        <f t="shared" si="1"/>
+        <v>5.7974441252655051E-3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="2">
+        <v>45198</v>
+      </c>
+      <c r="B97">
+        <v>427.48001099999999</v>
+      </c>
+      <c r="C97">
+        <f t="shared" si="1"/>
+        <v>-2.4269066244189119E-3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="2">
+        <v>45201</v>
+      </c>
+      <c r="B98">
+        <v>427.30999800000001</v>
+      </c>
+      <c r="C98">
+        <f t="shared" si="1"/>
+        <v>-3.9770982414422118E-4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="2">
+        <v>45202</v>
+      </c>
+      <c r="B99">
+        <v>421.58999599999999</v>
+      </c>
+      <c r="C99">
+        <f t="shared" si="1"/>
+        <v>-1.3386071064969585E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="2">
+        <v>45203</v>
+      </c>
+      <c r="B100">
+        <v>424.66000400000001</v>
+      </c>
+      <c r="C100">
+        <f t="shared" si="1"/>
+        <v>7.2819754480133447E-3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="2">
+        <v>45204</v>
+      </c>
+      <c r="B101">
+        <v>424.5</v>
+      </c>
+      <c r="C101">
+        <f t="shared" si="1"/>
+        <v>-3.7678142159114358E-4</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="2">
+        <v>45205</v>
+      </c>
+      <c r="B102">
+        <v>429.540009</v>
+      </c>
+      <c r="C102">
+        <f t="shared" si="1"/>
+        <v>1.1872812720848058E-2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="2">
+        <v>45208</v>
+      </c>
+      <c r="B103">
+        <v>432.290009</v>
+      </c>
+      <c r="C103">
+        <f t="shared" si="1"/>
+        <v>6.4021975657220231E-3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="2">
+        <v>45209</v>
+      </c>
+      <c r="B104">
+        <v>434.540009</v>
+      </c>
+      <c r="C104">
+        <f t="shared" si="1"/>
+        <v>5.2048392355974471E-3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="2">
+        <v>45210</v>
+      </c>
+      <c r="B105">
+        <v>436.32000699999998</v>
+      </c>
+      <c r="C105">
+        <f t="shared" si="1"/>
+        <v>4.0962810400273497E-3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="2">
+        <v>45211</v>
+      </c>
+      <c r="B106">
+        <v>433.66000400000001</v>
+      </c>
+      <c r="C106">
+        <f t="shared" si="1"/>
+        <v>-6.0964497555116015E-3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="2">
+        <v>45212</v>
+      </c>
+      <c r="B107">
+        <v>431.5</v>
+      </c>
+      <c r="C107">
+        <f t="shared" si="1"/>
+        <v>-4.9808697598960894E-3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="2">
+        <v>45215</v>
+      </c>
+      <c r="B108">
+        <v>436.040009</v>
+      </c>
+      <c r="C108">
+        <f t="shared" si="1"/>
+        <v>1.0521457705677806E-2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="2">
+        <v>45216</v>
+      </c>
+      <c r="B109">
+        <v>436.01998900000001</v>
+      </c>
+      <c r="C109">
+        <f t="shared" si="1"/>
+        <v>-4.5913218023052593E-5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="2">
+        <v>45217</v>
+      </c>
+      <c r="B110">
+        <v>430.209991</v>
+      </c>
+      <c r="C110">
+        <f t="shared" si="1"/>
+        <v>-1.3325072580560038E-2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="2">
+        <v>45218</v>
+      </c>
+      <c r="B111">
+        <v>426.42999300000002</v>
+      </c>
+      <c r="C111">
+        <f t="shared" si="1"/>
+        <v>-8.7864021735375442E-3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="2">
+        <v>45219</v>
+      </c>
+      <c r="B112">
+        <v>421.19000199999999</v>
+      </c>
+      <c r="C112">
+        <f t="shared" si="1"/>
+        <v>-1.2288045132885506E-2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="2">
+        <v>45222</v>
+      </c>
+      <c r="B113">
+        <v>420.459991</v>
+      </c>
+      <c r="C113">
+        <f t="shared" si="1"/>
+        <v>-1.7332106567904404E-3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="2">
+        <v>45223</v>
+      </c>
+      <c r="B114">
+        <v>423.63000499999998</v>
+      </c>
+      <c r="C114">
+        <f t="shared" si="1"/>
+        <v>7.5393951097715295E-3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="2">
+        <v>45224</v>
+      </c>
+      <c r="B115">
+        <v>417.54998799999998</v>
+      </c>
+      <c r="C115">
+        <f t="shared" si="1"/>
+        <v>-1.4352186880624784E-2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="2">
+        <v>45225</v>
+      </c>
+      <c r="B116">
+        <v>412.54998799999998</v>
+      </c>
+      <c r="C116">
+        <f t="shared" si="1"/>
+        <v>-1.1974614162843622E-2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="2">
+        <v>45226</v>
+      </c>
+      <c r="B117">
+        <v>410.67999300000002</v>
+      </c>
+      <c r="C117">
+        <f t="shared" si="1"/>
+        <v>-4.5327719170845659E-3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="2">
+        <v>45229</v>
+      </c>
+      <c r="B118">
+        <v>415.58999599999999</v>
+      </c>
+      <c r="C118">
+        <f t="shared" si="1"/>
+        <v>1.1955788165215031E-2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="2">
+        <v>45230</v>
+      </c>
+      <c r="B119">
+        <v>418.20001200000002</v>
+      </c>
+      <c r="C119">
+        <f t="shared" si="1"/>
+        <v>6.2802666693642095E-3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="2">
+        <v>45231</v>
+      </c>
+      <c r="B120">
+        <v>422.66000400000001</v>
+      </c>
+      <c r="C120">
+        <f t="shared" si="1"/>
+        <v>1.0664734270739329E-2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="2">
+        <v>45232</v>
+      </c>
+      <c r="B121">
+        <v>430.76001000000002</v>
+      </c>
+      <c r="C121">
+        <f t="shared" si="1"/>
+        <v>1.9164354145986273E-2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="2">
+        <v>45233</v>
+      </c>
+      <c r="B122">
+        <v>434.69000199999999</v>
+      </c>
+      <c r="C122">
+        <f t="shared" si="1"/>
+        <v>9.1233910037284982E-3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="2">
+        <v>45236</v>
+      </c>
+      <c r="B123">
+        <v>435.69000199999999</v>
+      </c>
+      <c r="C123">
+        <f t="shared" si="1"/>
+        <v>2.3004899937864032E-3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="2">
+        <v>45237</v>
+      </c>
+      <c r="B124">
+        <v>436.92999300000002</v>
+      </c>
+      <c r="C124">
+        <f t="shared" si="1"/>
+        <v>2.8460396022584877E-3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="2">
+        <v>45238</v>
+      </c>
+      <c r="B125">
+        <v>437.25</v>
+      </c>
+      <c r="C125">
+        <f t="shared" si="1"/>
+        <v>7.3239879414721543E-4</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="2">
+        <v>45239</v>
+      </c>
+      <c r="B126">
+        <v>433.83999599999999</v>
+      </c>
+      <c r="C126">
+        <f t="shared" si="1"/>
+        <v>-7.7987512864494679E-3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="2">
+        <v>45240</v>
+      </c>
+      <c r="B127">
+        <v>440.60998499999999</v>
+      </c>
+      <c r="C127">
+        <f t="shared" si="1"/>
+        <v>1.56048060631091E-2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="2">
+        <v>45243</v>
+      </c>
+      <c r="B128">
+        <v>440.19000199999999</v>
+      </c>
+      <c r="C128">
+        <f t="shared" si="1"/>
+        <v>-9.5318538911459694E-4</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="2">
+        <v>45244</v>
+      </c>
+      <c r="B129">
+        <v>448.73001099999999</v>
+      </c>
+      <c r="C129">
+        <f t="shared" si="1"/>
+        <v>1.9400733685905003E-2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="2">
+        <v>45245</v>
+      </c>
+      <c r="B130">
+        <v>449.67999300000002</v>
+      </c>
+      <c r="C130">
+        <f t="shared" si="1"/>
+        <v>2.1170458331569719E-3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="2">
+        <v>45246</v>
+      </c>
+      <c r="B131">
+        <v>450.23001099999999</v>
+      </c>
+      <c r="C131">
+        <f t="shared" si="1"/>
+        <v>1.2231320240212451E-3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="2">
+        <v>45247</v>
+      </c>
+      <c r="B132">
+        <v>450.790009</v>
+      </c>
+      <c r="C132">
+        <f t="shared" ref="C132:C195" si="2">B132/B131-1</f>
+        <v>1.2438042474249844E-3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="2">
+        <v>45250</v>
+      </c>
+      <c r="B133">
+        <v>454.26001000000002</v>
+      </c>
+      <c r="C133">
+        <f t="shared" si="2"/>
+        <v>7.6975996156116722E-3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="2">
+        <v>45251</v>
+      </c>
+      <c r="B134">
+        <v>453.26998900000001</v>
+      </c>
+      <c r="C134">
+        <f t="shared" si="2"/>
+        <v>-2.179414824562742E-3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="2">
+        <v>45252</v>
+      </c>
+      <c r="B135">
+        <v>455.01998900000001</v>
+      </c>
+      <c r="C135">
+        <f t="shared" si="2"/>
+        <v>3.860833592492785E-3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="2">
+        <v>45254</v>
+      </c>
+      <c r="B136">
+        <v>455.29998799999998</v>
+      </c>
+      <c r="C136">
+        <f t="shared" si="2"/>
+        <v>6.1535538387080813E-4</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="2">
+        <v>45257</v>
+      </c>
+      <c r="B137">
+        <v>454.48001099999999</v>
+      </c>
+      <c r="C137">
+        <f t="shared" si="2"/>
+        <v>-1.8009598541873784E-3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="2">
+        <v>45258</v>
+      </c>
+      <c r="B138">
+        <v>454.92999300000002</v>
+      </c>
+      <c r="C138">
+        <f t="shared" si="2"/>
+        <v>9.9010295086454647E-4</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="2">
+        <v>45259</v>
+      </c>
+      <c r="B139">
+        <v>454.60998499999999</v>
+      </c>
+      <c r="C139">
+        <f t="shared" si="2"/>
+        <v>-7.034225153847995E-4</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="2">
+        <v>45260</v>
+      </c>
+      <c r="B140">
+        <v>456.39999399999999</v>
+      </c>
+      <c r="C140">
+        <f t="shared" si="2"/>
+        <v>3.9374608105011699E-3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="2">
+        <v>45261</v>
+      </c>
+      <c r="B141">
+        <v>459.10000600000001</v>
+      </c>
+      <c r="C141">
+        <f t="shared" si="2"/>
+        <v>5.9158896483246792E-3</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" s="2">
+        <v>45264</v>
+      </c>
+      <c r="B142">
+        <v>456.69000199999999</v>
+      </c>
+      <c r="C142">
+        <f t="shared" si="2"/>
+        <v>-5.2494096460543593E-3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" s="2">
+        <v>45265</v>
+      </c>
+      <c r="B143">
+        <v>456.60000600000001</v>
+      </c>
+      <c r="C143">
+        <f t="shared" si="2"/>
+        <v>-1.9706146314979467E-4</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" s="2">
+        <v>45266</v>
+      </c>
+      <c r="B144">
+        <v>454.76001000000002</v>
+      </c>
+      <c r="C144">
+        <f t="shared" si="2"/>
+        <v>-4.0297765567702815E-3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" s="2">
+        <v>45267</v>
+      </c>
+      <c r="B145">
+        <v>458.23001099999999</v>
+      </c>
+      <c r="C145">
+        <f t="shared" si="2"/>
+        <v>7.6304004831031502E-3</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" s="2">
+        <v>45268</v>
+      </c>
+      <c r="B146">
+        <v>460.20001200000002</v>
+      </c>
+      <c r="C146">
+        <f t="shared" si="2"/>
+        <v>4.2991531604419375E-3</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" s="2">
+        <v>45271</v>
+      </c>
+      <c r="B147">
+        <v>461.98998999999998</v>
+      </c>
+      <c r="C147">
+        <f t="shared" si="2"/>
+        <v>3.8895653049222378E-3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" s="2">
+        <v>45272</v>
+      </c>
+      <c r="B148">
+        <v>464.10000600000001</v>
+      </c>
+      <c r="C148">
+        <f t="shared" si="2"/>
+        <v>4.5672331558526125E-3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" s="2">
+        <v>45273</v>
+      </c>
+      <c r="B149">
+        <v>470.5</v>
+      </c>
+      <c r="C149">
+        <f t="shared" si="2"/>
+        <v>1.3790118330659906E-2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" s="2">
+        <v>45274</v>
+      </c>
+      <c r="B150">
+        <v>472.01001000000002</v>
+      </c>
+      <c r="C150">
+        <f t="shared" si="2"/>
+        <v>3.2093730074389537E-3</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" s="2">
+        <v>45275</v>
+      </c>
+      <c r="B151">
+        <v>469.32998700000002</v>
+      </c>
+      <c r="C151">
+        <f t="shared" si="2"/>
+        <v>-5.6778944158408784E-3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" s="2">
+        <v>45278</v>
+      </c>
+      <c r="B152">
+        <v>471.97000100000002</v>
+      </c>
+      <c r="C152">
+        <f t="shared" si="2"/>
+        <v>5.6250699361342082E-3</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" s="2">
+        <v>45279</v>
+      </c>
+      <c r="B153">
+        <v>474.83999599999999</v>
+      </c>
+      <c r="C153">
+        <f t="shared" si="2"/>
+        <v>6.0808843653601397E-3</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" s="2">
+        <v>45280</v>
+      </c>
+      <c r="B154">
+        <v>468.26001000000002</v>
+      </c>
+      <c r="C154">
+        <f t="shared" si="2"/>
+        <v>-1.3857269933933658E-2</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" s="2">
+        <v>45281</v>
+      </c>
+      <c r="B155">
+        <v>472.70001200000002</v>
+      </c>
+      <c r="C155">
+        <f t="shared" si="2"/>
+        <v>9.4819158270635917E-3</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" s="2">
+        <v>45282</v>
+      </c>
+      <c r="B156">
+        <v>473.64999399999999</v>
+      </c>
+      <c r="C156">
+        <f t="shared" si="2"/>
+        <v>2.0096932005153612E-3</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" s="2">
+        <v>45286</v>
+      </c>
+      <c r="B157">
+        <v>475.64999399999999</v>
+      </c>
+      <c r="C157">
+        <f t="shared" si="2"/>
+        <v>4.2225272360079114E-3</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" s="2">
+        <v>45287</v>
+      </c>
+      <c r="B158">
+        <v>476.51001000000002</v>
+      </c>
+      <c r="C158">
+        <f t="shared" si="2"/>
+        <v>1.8080858001652267E-3</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" s="2">
+        <v>45288</v>
+      </c>
+      <c r="B159">
+        <v>476.69000199999999</v>
+      </c>
+      <c r="C159">
+        <f t="shared" si="2"/>
+        <v>3.777297354150555E-4</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" s="2">
+        <v>45289</v>
+      </c>
+      <c r="B160">
+        <v>475.30999800000001</v>
+      </c>
+      <c r="C160">
+        <f t="shared" si="2"/>
+        <v>-2.894971562671822E-3</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" s="2">
+        <v>45293</v>
+      </c>
+      <c r="B161">
+        <v>472.64999399999999</v>
+      </c>
+      <c r="C161">
+        <f t="shared" si="2"/>
+        <v>-5.5963560859075834E-3</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" s="2">
+        <v>45294</v>
+      </c>
+      <c r="B162">
+        <v>468.790009</v>
+      </c>
+      <c r="C162">
+        <f t="shared" si="2"/>
+        <v>-8.1666879276423021E-3</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" s="2">
+        <v>45295</v>
+      </c>
+      <c r="B163">
+        <v>467.27999899999998</v>
+      </c>
+      <c r="C163">
+        <f t="shared" si="2"/>
+        <v>-3.2210797393509294E-3</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" s="2">
+        <v>45296</v>
+      </c>
+      <c r="B164">
+        <v>467.92001299999998</v>
+      </c>
+      <c r="C164">
+        <f t="shared" si="2"/>
+        <v>1.369658451826794E-3</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" s="2">
+        <v>45299</v>
+      </c>
+      <c r="B165">
+        <v>474.60000600000001</v>
+      </c>
+      <c r="C165">
+        <f t="shared" si="2"/>
+        <v>1.4275929249472075E-2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" s="2">
+        <v>45300</v>
+      </c>
+      <c r="B166">
+        <v>473.88000499999998</v>
+      </c>
+      <c r="C166">
+        <f t="shared" si="2"/>
+        <v>-1.5170690916510576E-3</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" s="2">
+        <v>45301</v>
+      </c>
+      <c r="B167">
+        <v>476.55999800000001</v>
+      </c>
+      <c r="C167">
+        <f t="shared" si="2"/>
+        <v>5.6554253644864882E-3</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" s="2">
+        <v>45302</v>
+      </c>
+      <c r="B168">
+        <v>476.35000600000001</v>
+      </c>
+      <c r="C168">
+        <f t="shared" si="2"/>
+        <v>-4.4064126422960204E-4</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" s="2">
+        <v>45303</v>
+      </c>
+      <c r="B169">
+        <v>476.67999300000002</v>
+      </c>
+      <c r="C169">
+        <f t="shared" si="2"/>
+        <v>6.9274062316271312E-4</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" s="2">
+        <v>45307</v>
+      </c>
+      <c r="B170">
+        <v>474.92999300000002</v>
+      </c>
+      <c r="C170">
+        <f t="shared" si="2"/>
+        <v>-3.67122603360448E-3</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" s="2">
+        <v>45308</v>
+      </c>
+      <c r="B171">
+        <v>472.290009</v>
+      </c>
+      <c r="C171">
+        <f t="shared" si="2"/>
+        <v>-5.5586803084892722E-3</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" s="2">
+        <v>45309</v>
+      </c>
+      <c r="B172">
+        <v>476.48998999999998</v>
+      </c>
+      <c r="C172">
+        <f t="shared" si="2"/>
+        <v>8.8928008638013978E-3</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" s="2">
+        <v>45310</v>
+      </c>
+      <c r="B173">
+        <v>482.42999300000002</v>
+      </c>
+      <c r="C173">
+        <f t="shared" si="2"/>
+        <v>1.2466165343788305E-2</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" s="2">
+        <v>45313</v>
+      </c>
+      <c r="B174">
+        <v>483.45001200000002</v>
+      </c>
+      <c r="C174">
+        <f t="shared" si="2"/>
+        <v>2.1143357892343673E-3</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" s="2">
+        <v>45314</v>
+      </c>
+      <c r="B175">
+        <v>484.85998499999999</v>
+      </c>
+      <c r="C175">
+        <f t="shared" si="2"/>
+        <v>2.9164814665472161E-3</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" s="2">
+        <v>45315</v>
+      </c>
+      <c r="B176">
+        <v>485.39001500000001</v>
+      </c>
+      <c r="C176">
+        <f t="shared" si="2"/>
+        <v>1.0931609462472291E-3</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" s="2">
+        <v>45316</v>
+      </c>
+      <c r="B177">
+        <v>488.02999899999998</v>
+      </c>
+      <c r="C177">
+        <f t="shared" si="2"/>
+        <v>5.4388922689312391E-3</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" s="2">
+        <v>45317</v>
+      </c>
+      <c r="B178">
+        <v>487.41000400000001</v>
+      </c>
+      <c r="C178">
+        <f t="shared" si="2"/>
+        <v>-1.2704034614068327E-3</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" s="2">
+        <v>45320</v>
+      </c>
+      <c r="B179">
+        <v>491.26998900000001</v>
+      </c>
+      <c r="C179">
+        <f t="shared" si="2"/>
+        <v>7.9193799231087603E-3</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" s="2">
+        <v>45321</v>
+      </c>
+      <c r="B180">
+        <v>490.89001500000001</v>
+      </c>
+      <c r="C180">
+        <f t="shared" si="2"/>
+        <v>-7.7345249762450496E-4</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" s="2">
+        <v>45322</v>
+      </c>
+      <c r="B181">
+        <v>482.88000499999998</v>
+      </c>
+      <c r="C181">
+        <f t="shared" si="2"/>
+        <v>-1.631732110093953E-2</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" s="2">
+        <v>45323</v>
+      </c>
+      <c r="B182">
+        <v>489.20001200000002</v>
+      </c>
+      <c r="C182">
+        <f t="shared" si="2"/>
+        <v>1.3088152200462444E-2</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183" s="2">
+        <v>45324</v>
+      </c>
+      <c r="B183">
+        <v>494.35000600000001</v>
+      </c>
+      <c r="C183">
+        <f t="shared" si="2"/>
+        <v>1.0527379136695547E-2</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184" s="2">
+        <v>45327</v>
+      </c>
+      <c r="B184">
+        <v>492.54998799999998</v>
+      </c>
+      <c r="C184">
+        <f t="shared" si="2"/>
+        <v>-3.6411813050529762E-3</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" s="2">
+        <v>45328</v>
+      </c>
+      <c r="B185">
+        <v>493.98001099999999</v>
+      </c>
+      <c r="C185">
+        <f t="shared" si="2"/>
+        <v>2.9033053189313485E-3</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186" s="2">
+        <v>45329</v>
+      </c>
+      <c r="B186">
+        <v>498.10000600000001</v>
+      </c>
+      <c r="C186">
+        <f t="shared" si="2"/>
+        <v>8.3404083328384448E-3</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" s="2">
+        <v>45330</v>
+      </c>
+      <c r="B187">
+        <v>498.32000699999998</v>
+      </c>
+      <c r="C187">
+        <f t="shared" si="2"/>
+        <v>4.4168038014436029E-4</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" s="2">
+        <v>45331</v>
+      </c>
+      <c r="B188">
+        <v>501.20001200000002</v>
+      </c>
+      <c r="C188">
+        <f t="shared" si="2"/>
+        <v>5.7794287998556015E-3</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" s="2">
+        <v>45334</v>
+      </c>
+      <c r="B189">
+        <v>500.98001099999999</v>
+      </c>
+      <c r="C189">
+        <f t="shared" si="2"/>
+        <v>-4.3894851303405424E-4</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190" s="2">
+        <v>45335</v>
+      </c>
+      <c r="B190">
+        <v>494.07998700000002</v>
+      </c>
+      <c r="C190">
+        <f t="shared" si="2"/>
+        <v>-1.3773052514065243E-2</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191" s="2">
+        <v>45336</v>
+      </c>
+      <c r="B191">
+        <v>498.57000699999998</v>
+      </c>
+      <c r="C191">
+        <f t="shared" si="2"/>
+        <v>9.0876378686433057E-3</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192" s="2">
+        <v>45337</v>
+      </c>
+      <c r="B192">
+        <v>502.01001000000002</v>
+      </c>
+      <c r="C192">
+        <f t="shared" si="2"/>
+        <v>6.8997391573939471E-3</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193" s="2">
+        <v>45338</v>
+      </c>
+      <c r="B193">
+        <v>499.51001000000002</v>
+      </c>
+      <c r="C193">
+        <f t="shared" si="2"/>
+        <v>-4.9799803792757169E-3</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A194" s="2">
+        <v>45342</v>
+      </c>
+      <c r="B194">
+        <v>496.76001000000002</v>
+      </c>
+      <c r="C194">
+        <f t="shared" si="2"/>
+        <v>-5.5053951771657506E-3</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A195" s="2">
+        <v>45343</v>
+      </c>
+      <c r="B195">
+        <v>497.209991</v>
+      </c>
+      <c r="C195">
+        <f t="shared" si="2"/>
+        <v>9.058317717642872E-4</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A196" s="2">
+        <v>45344</v>
+      </c>
+      <c r="B196">
+        <v>507.5</v>
+      </c>
+      <c r="C196">
+        <f t="shared" ref="C196:C254" si="3">B196/B195-1</f>
+        <v>2.0695499258380767E-2</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A197" s="2">
+        <v>45345</v>
+      </c>
+      <c r="B197">
+        <v>507.85000600000001</v>
+      </c>
+      <c r="C197">
+        <f t="shared" si="3"/>
+        <v>6.8966699507400087E-4</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A198" s="2">
+        <v>45348</v>
+      </c>
+      <c r="B198">
+        <v>505.98998999999998</v>
+      </c>
+      <c r="C198">
+        <f t="shared" si="3"/>
+        <v>-3.6625302314164943E-3</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A199" s="2">
+        <v>45349</v>
+      </c>
+      <c r="B199">
+        <v>506.92999300000002</v>
+      </c>
+      <c r="C199">
+        <f t="shared" si="3"/>
+        <v>1.8577501898804361E-3</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A200" s="2">
+        <v>45350</v>
+      </c>
+      <c r="B200">
+        <v>506.26001000000002</v>
+      </c>
+      <c r="C200">
+        <f t="shared" si="3"/>
+        <v>-1.3216479775344236E-3</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A201" s="2">
+        <v>45351</v>
+      </c>
+      <c r="B201">
+        <v>508.07998700000002</v>
+      </c>
+      <c r="C201">
+        <f t="shared" si="3"/>
+        <v>3.5949452140215943E-3</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A202" s="2">
+        <v>45352</v>
+      </c>
+      <c r="B202">
+        <v>512.84997599999997</v>
+      </c>
+      <c r="C202">
+        <f t="shared" si="3"/>
+        <v>9.3882638994791101E-3</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A203" s="2">
+        <v>45355</v>
+      </c>
+      <c r="B203">
+        <v>512.29998799999998</v>
+      </c>
+      <c r="C203">
+        <f t="shared" si="3"/>
+        <v>-1.0724149863272636E-3</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A204" s="2">
+        <v>45356</v>
+      </c>
+      <c r="B204">
+        <v>507.17999300000002</v>
+      </c>
+      <c r="C204">
+        <f t="shared" si="3"/>
+        <v>-9.9941345304110918E-3</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A205" s="2">
+        <v>45357</v>
+      </c>
+      <c r="B205">
+        <v>509.75</v>
+      </c>
+      <c r="C205">
+        <f t="shared" si="3"/>
+        <v>5.0672483841451843E-3</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A206" s="2">
+        <v>45358</v>
+      </c>
+      <c r="B206">
+        <v>514.80999799999995</v>
+      </c>
+      <c r="C206">
+        <f t="shared" si="3"/>
+        <v>9.9264306032367244E-3</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A207" s="2">
+        <v>45359</v>
+      </c>
+      <c r="B207">
+        <v>511.72000100000002</v>
+      </c>
+      <c r="C207">
+        <f t="shared" si="3"/>
+        <v>-6.0022086051249035E-3</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A208" s="2">
+        <v>45362</v>
+      </c>
+      <c r="B208">
+        <v>511.27999899999998</v>
+      </c>
+      <c r="C208">
+        <f t="shared" si="3"/>
+        <v>-8.5984913456615963E-4</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A209" s="2">
+        <v>45363</v>
+      </c>
+      <c r="B209">
+        <v>516.78002900000001</v>
+      </c>
+      <c r="C209">
+        <f t="shared" si="3"/>
+        <v>1.0757373671486103E-2</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A210" s="2">
+        <v>45364</v>
+      </c>
+      <c r="B210">
+        <v>515.96997099999999</v>
+      </c>
+      <c r="C210">
+        <f t="shared" si="3"/>
+        <v>-1.5675102646043326E-3</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A211" s="2">
+        <v>45365</v>
+      </c>
+      <c r="B211">
+        <v>514.95001200000002</v>
+      </c>
+      <c r="C211">
+        <f t="shared" si="3"/>
+        <v>-1.9767797688364785E-3</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A212" s="2">
+        <v>45366</v>
+      </c>
+      <c r="B212">
+        <v>509.82998700000002</v>
+      </c>
+      <c r="C212">
+        <f t="shared" si="3"/>
+        <v>-9.942761201450323E-3</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A213" s="2">
+        <v>45369</v>
+      </c>
+      <c r="B213">
+        <v>512.85998500000005</v>
+      </c>
+      <c r="C213">
+        <f t="shared" si="3"/>
+        <v>5.9431537517624644E-3</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A214" s="2">
+        <v>45370</v>
+      </c>
+      <c r="B214">
+        <v>515.71002199999998</v>
+      </c>
+      <c r="C214">
+        <f t="shared" si="3"/>
+        <v>5.5571444124264957E-3</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A215" s="2">
+        <v>45371</v>
+      </c>
+      <c r="B215">
+        <v>520.47997999999995</v>
+      </c>
+      <c r="C215">
+        <f t="shared" si="3"/>
+        <v>9.2493025082223124E-3</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A216" s="2">
+        <v>45372</v>
+      </c>
+      <c r="B216">
+        <v>522.20001200000002</v>
+      </c>
+      <c r="C216">
+        <f t="shared" si="3"/>
+        <v>3.3047034777400341E-3</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A217" s="2">
+        <v>45373</v>
+      </c>
+      <c r="B217">
+        <v>521.21002199999998</v>
+      </c>
+      <c r="C217">
+        <f t="shared" si="3"/>
+        <v>-1.8958061609543053E-3</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A218" s="2">
+        <v>45376</v>
+      </c>
+      <c r="B218">
+        <v>519.77002000000005</v>
+      </c>
+      <c r="C218">
+        <f t="shared" si="3"/>
+        <v>-2.7628056622440722E-3</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A219" s="2">
+        <v>45377</v>
+      </c>
+      <c r="B219">
+        <v>518.80999799999995</v>
+      </c>
+      <c r="C219">
+        <f t="shared" si="3"/>
+        <v>-1.8470130308787525E-3</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A220" s="2">
+        <v>45378</v>
+      </c>
+      <c r="B220">
+        <v>523.169983</v>
+      </c>
+      <c r="C220">
+        <f t="shared" si="3"/>
+        <v>8.4038183859365123E-3</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A221" s="2">
+        <v>45379</v>
+      </c>
+      <c r="B221">
+        <v>523.07000700000003</v>
+      </c>
+      <c r="C221">
+        <f t="shared" si="3"/>
+        <v>-1.910965904937667E-4</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A222" s="2">
+        <v>45383</v>
+      </c>
+      <c r="B222">
+        <v>522.15997300000004</v>
+      </c>
+      <c r="C222">
+        <f t="shared" si="3"/>
+        <v>-1.7397938857541817E-3</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A223" s="2">
+        <v>45384</v>
+      </c>
+      <c r="B223">
+        <v>518.84002699999996</v>
+      </c>
+      <c r="C223">
+        <f t="shared" si="3"/>
+        <v>-6.358101293988061E-3</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A224" s="2">
+        <v>45385</v>
+      </c>
+      <c r="B224">
+        <v>519.40997300000004</v>
+      </c>
+      <c r="C224">
+        <f t="shared" si="3"/>
+        <v>1.0985004439529877E-3</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A225" s="2">
+        <v>45386</v>
+      </c>
+      <c r="B225">
+        <v>513.07000700000003</v>
+      </c>
+      <c r="C225">
+        <f t="shared" si="3"/>
+        <v>-1.2206092161422544E-2</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A226" s="2">
+        <v>45387</v>
+      </c>
+      <c r="B226">
+        <v>518.42999299999997</v>
+      </c>
+      <c r="C226">
+        <f t="shared" si="3"/>
+        <v>1.0446890145344057E-2</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A227" s="2">
+        <v>45390</v>
+      </c>
+      <c r="B227">
+        <v>518.71997099999999</v>
+      </c>
+      <c r="C227">
+        <f t="shared" si="3"/>
+        <v>5.5933878038572082E-4</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A228" s="2">
+        <v>45391</v>
+      </c>
+      <c r="B228">
+        <v>519.32000700000003</v>
+      </c>
+      <c r="C228">
+        <f t="shared" si="3"/>
+        <v>1.1567628654114426E-3</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A229" s="2">
+        <v>45392</v>
+      </c>
+      <c r="B229">
+        <v>514.11999500000002</v>
+      </c>
+      <c r="C229">
+        <f t="shared" si="3"/>
+        <v>-1.0013117018231932E-2</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A230" s="2">
+        <v>45393</v>
+      </c>
+      <c r="B230">
+        <v>518</v>
+      </c>
+      <c r="C230">
+        <f t="shared" si="3"/>
+        <v>7.546886014421661E-3</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A231" s="2">
+        <v>45394</v>
+      </c>
+      <c r="B231">
+        <v>510.85000600000001</v>
+      </c>
+      <c r="C231">
+        <f t="shared" si="3"/>
+        <v>-1.3803077220077231E-2</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A232" s="2">
+        <v>45397</v>
+      </c>
+      <c r="B232">
+        <v>504.45001200000002</v>
+      </c>
+      <c r="C232">
+        <f t="shared" si="3"/>
+        <v>-1.2528127483275364E-2</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A233" s="2">
+        <v>45398</v>
+      </c>
+      <c r="B233">
+        <v>503.52999899999998</v>
+      </c>
+      <c r="C233">
+        <f t="shared" si="3"/>
+        <v>-1.8237941879561959E-3</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A234" s="2">
+        <v>45399</v>
+      </c>
+      <c r="B234">
+        <v>500.54998799999998</v>
+      </c>
+      <c r="C234">
+        <f t="shared" si="3"/>
+        <v>-5.9182392427824526E-3</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A235" s="2">
+        <v>45400</v>
+      </c>
+      <c r="B235">
+        <v>499.51998900000001</v>
+      </c>
+      <c r="C235">
+        <f t="shared" si="3"/>
+        <v>-2.0577345413900217E-3</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A236" s="2">
+        <v>45401</v>
+      </c>
+      <c r="B236">
+        <v>495.16000400000001</v>
+      </c>
+      <c r="C236">
+        <f t="shared" si="3"/>
+        <v>-8.7283494074548162E-3</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A237" s="2">
+        <v>45404</v>
+      </c>
+      <c r="B237">
+        <v>499.72000100000002</v>
+      </c>
+      <c r="C237">
+        <f t="shared" si="3"/>
+        <v>9.2091383859025377E-3</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A238" s="2">
+        <v>45405</v>
+      </c>
+      <c r="B238">
+        <v>505.64999399999999</v>
+      </c>
+      <c r="C238">
+        <f t="shared" si="3"/>
+        <v>1.1866631289789042E-2</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A239" s="2">
+        <v>45406</v>
+      </c>
+      <c r="B239">
+        <v>505.41000400000001</v>
+      </c>
+      <c r="C239">
+        <f t="shared" si="3"/>
+        <v>-4.7461683545468869E-4</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A240" s="2">
+        <v>45407</v>
+      </c>
+      <c r="B240">
+        <v>503.48998999999998</v>
+      </c>
+      <c r="C240">
+        <f t="shared" si="3"/>
+        <v>-3.7989236160826945E-3</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A241" s="2">
+        <v>45408</v>
+      </c>
+      <c r="B241">
+        <v>508.26001000000002</v>
+      </c>
+      <c r="C241">
+        <f t="shared" si="3"/>
+        <v>9.4739122817517618E-3</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A242" s="2">
+        <v>45411</v>
+      </c>
+      <c r="B242">
+        <v>510.05999800000001</v>
+      </c>
+      <c r="C242">
+        <f t="shared" si="3"/>
+        <v>3.5414708310417264E-3</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A243" s="2">
+        <v>45412</v>
+      </c>
+      <c r="B243">
+        <v>501.98001099999999</v>
+      </c>
+      <c r="C243">
+        <f t="shared" si="3"/>
+        <v>-1.5841248150575415E-2</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A244" s="2">
+        <v>45413</v>
+      </c>
+      <c r="B244">
+        <v>500.35000600000001</v>
+      </c>
+      <c r="C244">
+        <f t="shared" si="3"/>
+        <v>-3.2471512097719257E-3</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A245" s="2">
+        <v>45414</v>
+      </c>
+      <c r="B245">
+        <v>505.02999899999998</v>
+      </c>
+      <c r="C245">
+        <f t="shared" si="3"/>
+        <v>9.3534384808220405E-3</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A246" s="2">
+        <v>45415</v>
+      </c>
+      <c r="B246">
+        <v>511.290009</v>
+      </c>
+      <c r="C246">
+        <f t="shared" si="3"/>
+        <v>1.2395323074659625E-2</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A247" s="2">
+        <v>45418</v>
+      </c>
+      <c r="B247">
+        <v>516.57000700000003</v>
+      </c>
+      <c r="C247">
+        <f t="shared" si="3"/>
+        <v>1.0326816302017816E-2</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A248" s="2">
+        <v>45419</v>
+      </c>
+      <c r="B248">
+        <v>517.14001499999995</v>
+      </c>
+      <c r="C248">
+        <f t="shared" si="3"/>
+        <v>1.1034477268827558E-3</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A249" s="2">
+        <v>45420</v>
+      </c>
+      <c r="B249">
+        <v>517.19000200000005</v>
+      </c>
+      <c r="C249">
+        <f t="shared" si="3"/>
+        <v>9.6660475983778582E-5</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A250" s="2">
+        <v>45421</v>
+      </c>
+      <c r="B250">
+        <v>520.169983</v>
+      </c>
+      <c r="C250">
+        <f t="shared" si="3"/>
+        <v>5.7618689233671638E-3</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A251" s="2">
+        <v>45422</v>
+      </c>
+      <c r="B251">
+        <v>520.84002699999996</v>
+      </c>
+      <c r="C251">
+        <f t="shared" si="3"/>
+        <v>1.2881250781437981E-3</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A252" s="2">
+        <v>45425</v>
+      </c>
+      <c r="B252">
+        <v>520.90997300000004</v>
+      </c>
+      <c r="C252">
+        <f t="shared" si="3"/>
+        <v>1.3429459406744115E-4</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A253" s="2">
+        <v>45426</v>
+      </c>
+      <c r="B253">
+        <v>523.29998799999998</v>
+      </c>
+      <c r="C253">
+        <f t="shared" si="3"/>
+        <v>4.5881536616307894E-3</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A254" s="2">
+        <v>45427</v>
+      </c>
+      <c r="B254">
+        <v>529.78</v>
+      </c>
+      <c r="C254">
+        <f t="shared" si="3"/>
+        <v>1.2382977543657026E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{984B722E-14BC-41ED-98D8-CD834162C366}">
   <dimension ref="A1:H254"/>
   <sheetViews>
-    <sheetView topLeftCell="A244" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11342,7 +14419,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FD67662-867E-45E7-91BE-793F81151AA3}">
   <dimension ref="A1:D254"/>
   <sheetViews>
@@ -15412,7 +18489,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21DD955D-7B94-48AA-AB94-C4BF390EB9F0}">
   <dimension ref="A1:D254"/>
   <sheetViews>

</xml_diff>